<commit_message>
92425 Funding summary report headers dynamic on collection year and report refactoring
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.NCS/ESFA.DC.NCS.ReportingService/Templates/FundingSummaryReportTemplate.xlsx
+++ b/src/ESFA.DC.NCS/ESFA.DC.NCS.ReportingService/Templates/FundingSummaryReportTemplate.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02ECEBBE-8A66-45EE-8BAD-65410DC18E55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F16CF58-8A67-4B3C-978B-C6D8E764063B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,13 +26,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="7">
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>Numbers</t>
-  </si>
-  <si>
-    <t>In Community Outcomes</t>
   </si>
   <si>
     <t xml:space="preserve">Total In Community Priority Group Outcomes </t>
@@ -45,6 +39,12 @@
   </si>
   <si>
     <t>Funding (£)</t>
+  </si>
+  <si>
+    <t>In Community Outcomes</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -857,140 +857,116 @@
     </row>
     <row r="6" spans="1:28" ht="16.899999999999999" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="21">
-        <v>43556</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B6" s="21"/>
       <c r="C6" s="22"/>
-      <c r="D6" s="21">
-        <v>43586</v>
-      </c>
+      <c r="D6" s="21"/>
       <c r="E6" s="22"/>
-      <c r="F6" s="21">
-        <v>43617</v>
-      </c>
+      <c r="F6" s="21"/>
       <c r="G6" s="22"/>
-      <c r="H6" s="21">
-        <v>43647</v>
-      </c>
+      <c r="H6" s="21"/>
       <c r="I6" s="22"/>
-      <c r="J6" s="21">
-        <v>43678</v>
-      </c>
+      <c r="J6" s="21"/>
       <c r="K6" s="22"/>
-      <c r="L6" s="21">
-        <v>43709</v>
-      </c>
+      <c r="L6" s="21"/>
       <c r="M6" s="22"/>
-      <c r="N6" s="21">
-        <v>43739</v>
-      </c>
+      <c r="N6" s="21"/>
       <c r="O6" s="22"/>
-      <c r="P6" s="21">
-        <v>43770</v>
-      </c>
+      <c r="P6" s="21"/>
       <c r="Q6" s="22"/>
-      <c r="R6" s="21">
-        <v>43800</v>
-      </c>
+      <c r="R6" s="21"/>
       <c r="S6" s="22"/>
-      <c r="T6" s="21">
-        <v>43831</v>
-      </c>
+      <c r="T6" s="21"/>
       <c r="U6" s="22"/>
-      <c r="V6" s="21">
-        <v>43862</v>
-      </c>
+      <c r="V6" s="21"/>
       <c r="W6" s="22"/>
-      <c r="X6" s="21">
-        <v>43891</v>
-      </c>
+      <c r="X6" s="21"/>
       <c r="Y6" s="22"/>
       <c r="Z6" s="21" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AA6" s="22"/>
     </row>
     <row r="7" spans="1:28" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A7" s="10"/>
       <c r="B7" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="N7" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P7" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S7" s="11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="T7" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U7" s="11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="V7" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W7" s="11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="X7" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y7" s="11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Z7" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA7" s="11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.35">
@@ -1140,7 +1116,7 @@
     </row>
     <row r="13" spans="1:28" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B13" s="10">
         <f t="shared" ref="B13:AA13" si="0">SUM(B8:B12)</f>
@@ -1395,7 +1371,7 @@
     </row>
     <row r="19" spans="1:27" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B19" s="10">
         <f>SUM(B14:B18)</f>
@@ -1504,7 +1480,7 @@
     </row>
     <row r="20" spans="1:27" ht="16.899999999999999" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B20" s="13">
         <f t="shared" ref="B20:AA20" si="2">SUM(B13,B19)</f>

</xml_diff>